<commit_message>
# sizing coef sécu -> ok #stand by loss conv -> ok # read droop curve -> OK # not cable sizing et conv -> ok
</commit_message>
<xml_diff>
--- a/grid_data_input_file_WIP_v1.xlsx
+++ b/grid_data_input_file_WIP_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c30483\Documents\dc_design_tool\dc_design_tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C821B69-D49D-4F56-82ED-6FBFFE3B91FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D4F32B-D595-4F89-89A2-EF7294A0FD08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="simple example" sheetId="20" r:id="rId1"/>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="294">
   <si>
     <t>Node_i</t>
   </si>
@@ -674,9 +674,6 @@
   </si>
   <si>
     <t>Line length (m)</t>
-  </si>
-  <si>
-    <t>Cable section (mm²)</t>
   </si>
   <si>
     <t>Maximum power (kW)</t>
@@ -1371,6 +1368,12 @@
   </si>
   <si>
     <t>[1.085; 0], [1; 1], [1; 1], [1; 1], [1; 1], [0.915; 1]</t>
+  </si>
+  <si>
+    <t>Cable R_km (Ohm/km)</t>
+  </si>
+  <si>
+    <t>Imax (A)</t>
   </si>
 </sst>
 </file>
@@ -45347,16 +45350,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>139220</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>357882</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>78578</xdr:rowOff>
+      <xdr:rowOff>71952</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>342314</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>560975</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>148215</xdr:rowOff>
+      <xdr:rowOff>141590</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -45379,8 +45382,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3767003" y="255274"/>
-          <a:ext cx="6265963" cy="3240633"/>
+          <a:off x="4651586" y="423135"/>
+          <a:ext cx="6166572" cy="3170646"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -45770,7 +45773,7 @@
     <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
       <c r="B2" s="73" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C2" s="73"/>
       <c r="D2" s="51"/>
@@ -45782,7 +45785,7 @@
     <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="51"/>
       <c r="B4" s="72" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C4" s="72"/>
       <c r="D4" s="51"/>
@@ -45790,7 +45793,7 @@
     <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="51"/>
       <c r="B5" s="71" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C5" s="71"/>
       <c r="D5" s="51"/>
@@ -45806,7 +45809,7 @@
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="51"/>
       <c r="B8" s="76" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C8" s="76"/>
       <c r="D8" s="51"/>
@@ -45814,7 +45817,7 @@
     <row r="9" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="51"/>
       <c r="B9" s="74" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C9" s="74"/>
       <c r="D9" s="51"/>
@@ -45822,7 +45825,7 @@
     <row r="10" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="51"/>
       <c r="B10" s="74" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C10" s="74"/>
       <c r="D10" s="51"/>
@@ -45830,7 +45833,7 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="51"/>
       <c r="B11" s="77" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C11" s="77"/>
       <c r="D11" s="51"/>
@@ -45838,7 +45841,7 @@
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="51"/>
       <c r="B12" s="74" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C12" s="74"/>
       <c r="D12" s="51"/>
@@ -45846,7 +45849,7 @@
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="51"/>
       <c r="B13" s="65" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C13" s="65"/>
       <c r="D13" s="56"/>
@@ -45866,7 +45869,7 @@
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="51"/>
       <c r="B16" s="76" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C16" s="76"/>
       <c r="D16" s="58"/>
@@ -45946,7 +45949,7 @@
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="51"/>
       <c r="B25" s="53" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C25" s="53"/>
       <c r="D25" s="58"/>
@@ -45954,7 +45957,7 @@
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="51"/>
       <c r="B26" s="70" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C26" s="70"/>
       <c r="D26" s="51"/>
@@ -45962,7 +45965,7 @@
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="51"/>
       <c r="B27" s="65" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C27" s="65"/>
       <c r="D27" s="51"/>
@@ -45970,7 +45973,7 @@
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="51"/>
       <c r="B28" s="67" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C28" s="67"/>
       <c r="D28" s="51"/>
@@ -45978,7 +45981,7 @@
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="51"/>
       <c r="B29" s="66" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C29" s="66"/>
       <c r="D29" s="51"/>
@@ -45986,18 +45989,18 @@
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="51"/>
       <c r="B30" s="65" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C30" s="65"/>
       <c r="D30" s="51"/>
       <c r="F30" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="51"/>
       <c r="B31" s="65" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C31" s="65"/>
       <c r="D31" s="51"/>
@@ -46005,7 +46008,7 @@
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="51"/>
       <c r="B32" s="67" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C32" s="67"/>
       <c r="D32" s="51"/>
@@ -46013,7 +46016,7 @@
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="51"/>
       <c r="B33" s="65" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C33" s="65"/>
       <c r="D33" s="51"/>
@@ -46025,7 +46028,7 @@
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="51"/>
       <c r="B35" s="70" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C35" s="70"/>
       <c r="D35" s="51"/>
@@ -46033,7 +46036,7 @@
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="51"/>
       <c r="B36" s="65" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C36" s="65"/>
       <c r="D36" s="51"/>
@@ -46041,7 +46044,7 @@
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="51"/>
       <c r="B37" s="65" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C37" s="65"/>
       <c r="D37" s="51"/>
@@ -46049,7 +46052,7 @@
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="51"/>
       <c r="B38" s="65" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C38" s="65"/>
       <c r="D38" s="51"/>
@@ -46057,7 +46060,7 @@
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="51"/>
       <c r="B39" s="65" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C39" s="65"/>
       <c r="D39" s="51"/>
@@ -46065,7 +46068,7 @@
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="51"/>
       <c r="B40" s="78" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C40" s="78"/>
       <c r="D40" s="51"/>
@@ -46073,7 +46076,7 @@
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="51"/>
       <c r="B41" s="65" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C41" s="65"/>
       <c r="D41" s="51"/>
@@ -46081,7 +46084,7 @@
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="51"/>
       <c r="B42" s="65" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C42" s="65"/>
       <c r="D42" s="51"/>
@@ -46089,7 +46092,7 @@
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="51"/>
       <c r="B43" s="65" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C43" s="65"/>
       <c r="D43" s="51"/>
@@ -46103,7 +46106,7 @@
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="51"/>
       <c r="B45" s="70" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C45" s="70"/>
       <c r="D45" s="51"/>
@@ -46111,7 +46114,7 @@
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="51"/>
       <c r="B46" s="65" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C46" s="65"/>
       <c r="D46" s="51"/>
@@ -46119,7 +46122,7 @@
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="51"/>
       <c r="B47" s="68" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C47" s="65"/>
       <c r="D47" s="51"/>
@@ -46127,7 +46130,7 @@
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="51"/>
       <c r="B48" s="65" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C48" s="65"/>
       <c r="D48" s="51"/>
@@ -46135,7 +46138,7 @@
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="51"/>
       <c r="B49" s="68" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C49" s="65"/>
       <c r="D49" s="51"/>
@@ -46143,7 +46146,7 @@
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="51"/>
       <c r="B50" s="65" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C50" s="65"/>
       <c r="D50" s="51"/>
@@ -46151,7 +46154,7 @@
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="51"/>
       <c r="B51" s="68" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C51" s="65"/>
       <c r="D51" s="51"/>
@@ -46159,7 +46162,7 @@
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="51"/>
       <c r="B52" s="65" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C52" s="65"/>
       <c r="D52" s="51"/>
@@ -46167,7 +46170,7 @@
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="51"/>
       <c r="B53" s="68" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C53" s="65"/>
       <c r="D53" s="51"/>
@@ -46175,7 +46178,7 @@
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="51"/>
       <c r="B54" s="65" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C54" s="65"/>
       <c r="D54" s="51"/>
@@ -46189,7 +46192,7 @@
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="51"/>
       <c r="B56" s="70" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C56" s="70"/>
       <c r="D56" s="51"/>
@@ -46197,7 +46200,7 @@
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="51"/>
       <c r="B57" s="65" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C57" s="65"/>
       <c r="D57" s="51"/>
@@ -46205,7 +46208,7 @@
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="51"/>
       <c r="B58" s="65" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C58" s="65"/>
       <c r="D58" s="51"/>
@@ -46225,7 +46228,7 @@
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="51"/>
       <c r="B61" s="70" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C61" s="70"/>
       <c r="D61" s="51"/>
@@ -46233,7 +46236,7 @@
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="51"/>
       <c r="B62" s="65" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C62" s="65"/>
       <c r="D62" s="51"/>
@@ -46241,7 +46244,7 @@
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="51"/>
       <c r="B63" s="65" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C63" s="65"/>
       <c r="D63" s="51"/>
@@ -46249,7 +46252,7 @@
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="51"/>
       <c r="B64" s="65" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C64" s="65"/>
       <c r="D64" s="51"/>
@@ -46257,7 +46260,7 @@
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="51"/>
       <c r="B65" s="65" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C65" s="65"/>
       <c r="D65" s="51"/>
@@ -46396,13 +46399,13 @@
         <v>62</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F2" s="35" t="s">
         <v>159</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H2" s="20" t="s">
         <v>68</v>
@@ -46425,7 +46428,7 @@
         <v>134</v>
       </c>
       <c r="G3" s="42" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H3" s="24"/>
       <c r="I3" s="60"/>
@@ -46445,10 +46448,10 @@
         <v>7</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G4" s="80" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H4" s="26"/>
       <c r="I4" s="60"/>
@@ -46484,7 +46487,7 @@
         <v>135</v>
       </c>
       <c r="G6" s="80" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="60"/>
@@ -46533,10 +46536,10 @@
         <v>10</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G10" s="80" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="60"/>
@@ -46547,7 +46550,7 @@
       <c r="C11" s="22"/>
       <c r="D11" s="81"/>
       <c r="E11" s="22" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F11" s="38"/>
       <c r="G11" s="81"/>
@@ -46572,7 +46575,7 @@
         <v>136</v>
       </c>
       <c r="G12" s="80" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="60"/>
@@ -46610,7 +46613,7 @@
       <c r="E15" s="22"/>
       <c r="F15" s="38"/>
       <c r="G15" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H15" s="21" t="s">
         <v>5</v>
@@ -46629,7 +46632,7 @@
       <c r="E16" s="22"/>
       <c r="F16" s="38"/>
       <c r="G16" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H16" s="21" t="s">
         <v>5</v>
@@ -46652,7 +46655,7 @@
         <v>137</v>
       </c>
       <c r="G17" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H17" s="28"/>
       <c r="I17" s="60"/>
@@ -46673,7 +46676,7 @@
         <v>138</v>
       </c>
       <c r="G18" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H18" s="28"/>
       <c r="I18" s="60"/>
@@ -46694,7 +46697,7 @@
         <v>139</v>
       </c>
       <c r="G19" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H19" s="28"/>
       <c r="I19" s="60"/>
@@ -46715,7 +46718,7 @@
         <v>140</v>
       </c>
       <c r="G20" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H20" s="28"/>
       <c r="I20" s="60"/>
@@ -46736,7 +46739,7 @@
         <v>141</v>
       </c>
       <c r="G21" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H21" s="28"/>
       <c r="I21" s="60"/>
@@ -46757,7 +46760,7 @@
         <v>143</v>
       </c>
       <c r="G22" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H22" s="28"/>
       <c r="I22" s="60"/>
@@ -46778,7 +46781,7 @@
         <v>142</v>
       </c>
       <c r="G23" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H23" s="28"/>
       <c r="I23" s="60"/>
@@ -46799,7 +46802,7 @@
         <v>145</v>
       </c>
       <c r="G24" s="36" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H24" s="28" t="s">
         <v>32</v>
@@ -46826,7 +46829,7 @@
         <v>146</v>
       </c>
       <c r="G25" s="80" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H25" s="26"/>
       <c r="I25" s="60"/>
@@ -46866,7 +46869,7 @@
         <v>147</v>
       </c>
       <c r="G27" s="80" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H27" s="26"/>
       <c r="I27" s="60"/>
@@ -46904,7 +46907,7 @@
         <v>150</v>
       </c>
       <c r="G29" s="36" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H29" s="28" t="s">
         <v>67</v>
@@ -46929,7 +46932,7 @@
         <v>151</v>
       </c>
       <c r="G30" s="39" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H30" s="28" t="s">
         <v>67</v>
@@ -46954,7 +46957,7 @@
         <v>150</v>
       </c>
       <c r="G31" s="36" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H31" s="28" t="s">
         <v>67</v>
@@ -46979,7 +46982,7 @@
         <v>150</v>
       </c>
       <c r="G32" s="36" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H32" s="28" t="s">
         <v>67</v>
@@ -47003,10 +47006,10 @@
         <v>132</v>
       </c>
       <c r="F33" s="39" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G33" s="80" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I33" s="60"/>
       <c r="K33" s="4"/>
@@ -47020,7 +47023,7 @@
         <v>133</v>
       </c>
       <c r="F34" s="39" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G34" s="81"/>
       <c r="I34" s="60"/>
@@ -47060,7 +47063,7 @@
         <v>155</v>
       </c>
       <c r="G36" s="84" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H36" s="31"/>
       <c r="I36" s="60"/>
@@ -47126,7 +47129,7 @@
         <v>156</v>
       </c>
       <c r="G42" s="36" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H42" s="28"/>
       <c r="I42" s="60"/>
@@ -47149,7 +47152,7 @@
         <v>116</v>
       </c>
       <c r="G43" s="80" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H43" s="26"/>
       <c r="I43" s="60"/>
@@ -47207,7 +47210,7 @@
         <v>158</v>
       </c>
       <c r="G47" s="36" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H47" s="28" t="s">
         <v>2</v>
@@ -47230,7 +47233,7 @@
         <v>160</v>
       </c>
       <c r="G48" s="36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H48" s="28" t="s">
         <v>5</v>
@@ -47253,7 +47256,7 @@
         <v>162</v>
       </c>
       <c r="G49" s="36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H49" s="28" t="s">
         <v>94</v>
@@ -47276,7 +47279,7 @@
         <v>168</v>
       </c>
       <c r="G50" s="36" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H50" s="28"/>
       <c r="I50" s="60"/>
@@ -47297,7 +47300,7 @@
         <v>167</v>
       </c>
       <c r="G51" s="36" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H51" s="28"/>
       <c r="I51" s="60"/>
@@ -47333,7 +47336,7 @@
         <v>168</v>
       </c>
       <c r="G53" s="42" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H53" s="24"/>
       <c r="I53" s="60"/>
@@ -47344,17 +47347,17 @@
         <v>57</v>
       </c>
       <c r="C54" s="29" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D54" s="36" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E54" s="29"/>
       <c r="F54" s="36" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G54" s="36" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H54" s="28"/>
       <c r="I54" s="60"/>
@@ -47365,17 +47368,17 @@
         <v>57</v>
       </c>
       <c r="C55" s="29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D55" s="36" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E55" s="29"/>
       <c r="F55" s="36" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G55" s="36" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H55" s="28"/>
       <c r="I55" s="60"/>
@@ -47392,13 +47395,13 @@
         <v>88</v>
       </c>
       <c r="E56" s="27" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F56" s="37" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G56" s="80" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H56" s="26"/>
       <c r="I56" s="60"/>
@@ -47406,7 +47409,7 @@
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="60"/>
       <c r="E57" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G57" s="65"/>
       <c r="I57" s="60"/>
@@ -47422,7 +47425,7 @@
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="60"/>
       <c r="E59" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G59" s="65"/>
       <c r="I59" s="60"/>
@@ -47430,7 +47433,7 @@
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="60"/>
       <c r="E60" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G60" s="65"/>
       <c r="I60" s="60"/>
@@ -47470,17 +47473,17 @@
         <v>57</v>
       </c>
       <c r="C64" s="29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D64" s="36" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E64" s="29"/>
       <c r="F64" s="36" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G64" s="36" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H64" s="28" t="s">
         <v>2</v>
@@ -47493,17 +47496,17 @@
         <v>57</v>
       </c>
       <c r="C65" s="29" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D65" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E65" s="29"/>
       <c r="F65" s="36" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G65" s="36" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H65" s="28" t="s">
         <v>2</v>
@@ -47519,14 +47522,14 @@
         <v>46</v>
       </c>
       <c r="D66" s="36" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E66" s="29"/>
       <c r="F66" s="36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G66" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H66" s="28" t="s">
         <v>5</v>
@@ -47542,16 +47545,16 @@
         <v>70</v>
       </c>
       <c r="D67" s="37" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E67" s="27" t="s">
         <v>39</v>
       </c>
       <c r="F67" s="39" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G67" s="80" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H67" s="26"/>
       <c r="I67" s="60"/>
@@ -47565,7 +47568,7 @@
         <v>125</v>
       </c>
       <c r="F68" s="38" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G68" s="81"/>
       <c r="H68" s="21"/>
@@ -47580,14 +47583,14 @@
         <v>124</v>
       </c>
       <c r="D69" s="38" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E69" s="29"/>
       <c r="F69" s="36" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G69" s="38" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H69" s="21"/>
       <c r="I69" s="60"/>
@@ -47601,16 +47604,16 @@
         <v>27</v>
       </c>
       <c r="D70" s="37" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>127</v>
       </c>
       <c r="F70" s="39" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G70" s="82" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H70" s="26"/>
       <c r="I70" s="60"/>
@@ -47637,26 +47640,26 @@
         <v>69</v>
       </c>
       <c r="D72" s="39" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E72" s="27" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F72" s="39" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G72" s="80" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I72" s="60"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="60"/>
       <c r="E73" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F73" s="39" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G73" s="65"/>
       <c r="I73" s="60"/>
@@ -47664,10 +47667,10 @@
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="60"/>
       <c r="E74" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F74" s="39" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G74" s="65"/>
       <c r="I74" s="60"/>
@@ -47678,10 +47681,10 @@
       <c r="C75" s="22"/>
       <c r="D75" s="38"/>
       <c r="E75" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F75" s="38" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G75" s="81"/>
       <c r="H75" s="21"/>
@@ -47696,14 +47699,14 @@
         <v>128</v>
       </c>
       <c r="D76" s="38" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E76" s="22"/>
       <c r="F76" s="36" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G76" s="38" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H76" s="21"/>
       <c r="I76" s="60"/>
@@ -47714,17 +47717,17 @@
         <v>59</v>
       </c>
       <c r="C77" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D77" s="38" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E77" s="22"/>
       <c r="F77" s="36" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G77" s="22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H77" s="32"/>
       <c r="I77" s="60"/>
@@ -47735,17 +47738,17 @@
         <v>59</v>
       </c>
       <c r="C78" s="29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D78" s="36" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E78" s="29"/>
       <c r="F78" s="36" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G78" s="29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H78" s="28"/>
       <c r="I78" s="60"/>
@@ -47763,10 +47766,10 @@
       </c>
       <c r="E79" s="29"/>
       <c r="F79" s="36" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G79" s="29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H79" s="28" t="s">
         <v>97</v>
@@ -47782,14 +47785,14 @@
         <v>171</v>
       </c>
       <c r="D80" s="38" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E80" s="22"/>
       <c r="F80" s="36" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G80" s="43" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H80" s="21" t="s">
         <v>123</v>
@@ -47850,8 +47853,8 @@
   </sheetPr>
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="88" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:B36"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" zoomScalePageLayoutView="88" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.19921875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -48261,7 +48264,7 @@
   </sheetPr>
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
@@ -48291,19 +48294,19 @@
         <v>85</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>13</v>
       </c>
       <c r="G1" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>218</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>219</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>29</v>
@@ -48674,19 +48677,19 @@
         <v>38</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>35</v>
       </c>
       <c r="E1" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>188</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>189</v>
       </c>
       <c r="G1" s="13" t="s">
         <v>46</v>
@@ -48695,7 +48698,7 @@
         <v>70</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>27</v>
@@ -48704,7 +48707,7 @@
         <v>69</v>
       </c>
       <c r="L1" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="27.6" x14ac:dyDescent="0.25">
@@ -48720,7 +48723,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E2" s="1">
         <v>400</v>
@@ -48735,16 +48738,16 @@
         <v>125</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J2" s="15" t="s">
         <v>127</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -48770,13 +48773,13 @@
         <v>39</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>127</v>
       </c>
       <c r="K3" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L3" s="15"/>
     </row>
@@ -48803,13 +48806,13 @@
         <v>39</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>127</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L4" s="15"/>
     </row>
@@ -48835,13 +48838,13 @@
         <v>39</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>127</v>
       </c>
       <c r="K5" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L5" s="15"/>
     </row>
@@ -48867,13 +48870,13 @@
         <v>39</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>127</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L6" s="15"/>
     </row>
@@ -48899,13 +48902,13 @@
         <v>39</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>127</v>
       </c>
       <c r="K7" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L7" s="15"/>
     </row>
@@ -48920,7 +48923,7 @@
         <v>17</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E8" s="2">
         <v>48</v>
@@ -48933,13 +48936,13 @@
         <v>39</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>127</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L8" s="15"/>
     </row>
@@ -48954,7 +48957,7 @@
         <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E9" s="2">
         <v>350</v>
@@ -48967,13 +48970,13 @@
         <v>39</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>127</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L9" s="15"/>
     </row>
@@ -49027,11 +49030,11 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.69921875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -49042,7 +49045,7 @@
     <col min="4" max="4" width="18" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -49053,10 +49056,13 @@
         <v>173</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>174</v>
+        <v>292</v>
+      </c>
+      <c r="E1" t="s">
+        <v>293</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -49067,8 +49073,9 @@
         <v>100</v>
       </c>
       <c r="D2" s="2"/>
+      <c r="E2" s="64"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -49080,7 +49087,7 @@
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -49092,7 +49099,7 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -49104,7 +49111,7 @@
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -49116,7 +49123,7 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -49128,7 +49135,7 @@
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -49140,7 +49147,7 @@
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>15</v>
       </c>
@@ -49152,7 +49159,7 @@
       </c>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>17</v>
       </c>
@@ -49164,7 +49171,7 @@
       </c>
       <c r="D10" s="9"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>18</v>
       </c>
@@ -49176,7 +49183,7 @@
       </c>
       <c r="D11" s="9"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>19</v>
       </c>
@@ -49188,7 +49195,7 @@
       </c>
       <c r="D12" s="9"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>20</v>
       </c>
@@ -49200,7 +49207,7 @@
       </c>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="64">
         <v>14</v>
       </c>
@@ -49212,13 +49219,13 @@
       </c>
       <c r="D14"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="64"/>
       <c r="B15" s="64"/>
       <c r="C15" s="64"/>
       <c r="D15"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
@@ -49364,7 +49371,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B1" s="46">
         <v>0</v>
@@ -49387,27 +49394,27 @@
         <v>35</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="C2" s="45" t="s">
         <v>226</v>
       </c>
-      <c r="C2" s="45" t="s">
-        <v>227</v>
-      </c>
       <c r="D2" s="45" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F2" s="45" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -49419,7 +49426,7 @@
         <v>89</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -49431,7 +49438,7 @@
         <v>91</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -49443,7 +49450,7 @@
         <v>92</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -49455,7 +49462,7 @@
         <v>92</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -49467,7 +49474,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -49476,10 +49483,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -49488,10 +49495,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>

</xml_diff>

<commit_message>
refactoring worst case sizing
</commit_message>
<xml_diff>
--- a/grid_data_input_file_WIP_v1.xlsx
+++ b/grid_data_input_file_WIP_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c30483\Documents\dc_design_tool\dc_design_tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799F50D2-8745-4EA0-9EA8-4D9BF7A3C292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5249EB1-373F-451A-A357-5B49410D98C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23196" yWindow="10692" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1661,29 +1661,23 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
@@ -1697,11 +1691,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2448,8 +2448,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2865966" y="3837460"/>
-          <a:ext cx="389297" cy="323457"/>
+          <a:off x="2877396" y="3759355"/>
+          <a:ext cx="391202" cy="317742"/>
           <a:chOff x="3573269" y="3601319"/>
           <a:chExt cx="424926" cy="329094"/>
         </a:xfrm>
@@ -2715,8 +2715,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2865966" y="2986499"/>
-          <a:ext cx="389297" cy="318643"/>
+          <a:off x="2877396" y="2923634"/>
+          <a:ext cx="391202" cy="312928"/>
           <a:chOff x="3573269" y="3601319"/>
           <a:chExt cx="424926" cy="329094"/>
         </a:xfrm>
@@ -3439,8 +3439,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2866797" y="1785849"/>
-          <a:ext cx="389297" cy="323457"/>
+          <a:off x="2878227" y="1745844"/>
+          <a:ext cx="391202" cy="319647"/>
           <a:chOff x="3573269" y="3601319"/>
           <a:chExt cx="424926" cy="329094"/>
         </a:xfrm>
@@ -3761,8 +3761,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2865966" y="4702230"/>
-          <a:ext cx="389297" cy="323457"/>
+          <a:off x="2877396" y="4601265"/>
+          <a:ext cx="391202" cy="319647"/>
           <a:chOff x="3573269" y="3601319"/>
           <a:chExt cx="424926" cy="329094"/>
         </a:xfrm>
@@ -7440,8 +7440,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5017782" y="1450175"/>
-          <a:ext cx="1424674" cy="749765"/>
+          <a:off x="5034927" y="1421600"/>
+          <a:ext cx="1436104" cy="728810"/>
           <a:chOff x="5974842" y="1887551"/>
           <a:chExt cx="1550251" cy="767591"/>
         </a:xfrm>
@@ -9187,8 +9187,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5665719" y="2946564"/>
-          <a:ext cx="385489" cy="323455"/>
+          <a:off x="5692389" y="2883699"/>
+          <a:ext cx="385489" cy="317740"/>
           <a:chOff x="3573266" y="3601319"/>
           <a:chExt cx="424929" cy="329093"/>
         </a:xfrm>
@@ -20926,8 +20926,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="0" y="563879"/>
-          <a:ext cx="11123295" cy="5490211"/>
+          <a:off x="0" y="552449"/>
+          <a:ext cx="11170920" cy="5368291"/>
           <a:chOff x="335486" y="881826"/>
           <a:chExt cx="12151247" cy="5595213"/>
         </a:xfrm>
@@ -45590,16 +45590,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="50"/>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
       <c r="D1" s="50"/>
     </row>
     <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="50"/>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="72" t="s">
         <v>267</v>
       </c>
-      <c r="C2" s="74"/>
+      <c r="C2" s="72"/>
       <c r="D2" s="50"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -45608,18 +45608,18 @@
     </row>
     <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="50"/>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="71" t="s">
         <v>254</v>
       </c>
-      <c r="C4" s="73"/>
+      <c r="C4" s="71"/>
       <c r="D4" s="50"/>
     </row>
     <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="50"/>
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="70" t="s">
         <v>255</v>
       </c>
-      <c r="C5" s="72"/>
+      <c r="C5" s="70"/>
       <c r="D5" s="50"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -45632,70 +45632,70 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="50"/>
-      <c r="B8" s="65" t="s">
+      <c r="B8" s="75" t="s">
         <v>224</v>
       </c>
-      <c r="C8" s="65"/>
+      <c r="C8" s="75"/>
       <c r="D8" s="50"/>
     </row>
     <row r="9" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="50"/>
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="73" t="s">
         <v>223</v>
       </c>
-      <c r="C9" s="75"/>
+      <c r="C9" s="73"/>
       <c r="D9" s="50"/>
     </row>
     <row r="10" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="50"/>
-      <c r="B10" s="75" t="s">
+      <c r="B10" s="73" t="s">
         <v>222</v>
       </c>
-      <c r="C10" s="75"/>
+      <c r="C10" s="73"/>
       <c r="D10" s="50"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="50"/>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="76" t="s">
         <v>226</v>
       </c>
-      <c r="C11" s="66"/>
+      <c r="C11" s="76"/>
       <c r="D11" s="50"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="50"/>
-      <c r="B12" s="75" t="s">
+      <c r="B12" s="73" t="s">
         <v>227</v>
       </c>
-      <c r="C12" s="75"/>
+      <c r="C12" s="73"/>
       <c r="D12" s="50"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="50"/>
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="64" t="s">
         <v>228</v>
       </c>
-      <c r="C13" s="67"/>
+      <c r="C13" s="64"/>
       <c r="D13" s="55"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="50"/>
-      <c r="B14" s="67"/>
-      <c r="C14" s="67"/>
+      <c r="B14" s="64"/>
+      <c r="C14" s="64"/>
       <c r="D14" s="56"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="50"/>
-      <c r="B15" s="67"/>
-      <c r="C15" s="67"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="64"/>
       <c r="D15" s="50"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="50"/>
-      <c r="B16" s="65" t="s">
+      <c r="B16" s="75" t="s">
         <v>225</v>
       </c>
-      <c r="C16" s="65"/>
+      <c r="C16" s="75"/>
       <c r="D16" s="57"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -45760,14 +45760,14 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="50"/>
-      <c r="B23" s="67"/>
-      <c r="C23" s="67"/>
+      <c r="B23" s="64"/>
+      <c r="C23" s="64"/>
       <c r="D23" s="50"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="50"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="67"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="64"/>
       <c r="D24" s="50"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -45780,42 +45780,42 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="50"/>
-      <c r="B26" s="70" t="s">
+      <c r="B26" s="69" t="s">
         <v>232</v>
       </c>
-      <c r="C26" s="70"/>
+      <c r="C26" s="69"/>
       <c r="D26" s="50"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="50"/>
-      <c r="B27" s="67" t="s">
+      <c r="B27" s="64" t="s">
         <v>231</v>
       </c>
-      <c r="C27" s="67"/>
+      <c r="C27" s="64"/>
       <c r="D27" s="50"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="50"/>
-      <c r="B28" s="77" t="s">
+      <c r="B28" s="66" t="s">
         <v>230</v>
       </c>
-      <c r="C28" s="77"/>
+      <c r="C28" s="66"/>
       <c r="D28" s="50"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="50"/>
-      <c r="B29" s="76" t="s">
+      <c r="B29" s="65" t="s">
         <v>234</v>
       </c>
-      <c r="C29" s="76"/>
+      <c r="C29" s="65"/>
       <c r="D29" s="50"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="50"/>
-      <c r="B30" s="67" t="s">
+      <c r="B30" s="64" t="s">
         <v>256</v>
       </c>
-      <c r="C30" s="67"/>
+      <c r="C30" s="64"/>
       <c r="D30" s="50"/>
       <c r="F30" t="s">
         <v>253</v>
@@ -45823,26 +45823,26 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="50"/>
-      <c r="B31" s="67" t="s">
+      <c r="B31" s="64" t="s">
         <v>257</v>
       </c>
-      <c r="C31" s="67"/>
+      <c r="C31" s="64"/>
       <c r="D31" s="50"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="50"/>
-      <c r="B32" s="77" t="s">
+      <c r="B32" s="66" t="s">
         <v>258</v>
       </c>
-      <c r="C32" s="77"/>
+      <c r="C32" s="66"/>
       <c r="D32" s="50"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="50"/>
-      <c r="B33" s="67" t="s">
+      <c r="B33" s="64" t="s">
         <v>259</v>
       </c>
-      <c r="C33" s="67"/>
+      <c r="C33" s="64"/>
       <c r="D33" s="50"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -45851,190 +45851,190 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="50"/>
-      <c r="B35" s="70" t="s">
+      <c r="B35" s="69" t="s">
         <v>269</v>
       </c>
-      <c r="C35" s="70"/>
+      <c r="C35" s="69"/>
       <c r="D35" s="50"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="50"/>
-      <c r="B36" s="67" t="s">
+      <c r="B36" s="64" t="s">
         <v>233</v>
       </c>
-      <c r="C36" s="67"/>
+      <c r="C36" s="64"/>
       <c r="D36" s="50"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="50"/>
-      <c r="B37" s="67" t="s">
+      <c r="B37" s="64" t="s">
         <v>260</v>
       </c>
-      <c r="C37" s="67"/>
+      <c r="C37" s="64"/>
       <c r="D37" s="50"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="50"/>
-      <c r="B38" s="67" t="s">
+      <c r="B38" s="64" t="s">
         <v>261</v>
       </c>
-      <c r="C38" s="67"/>
+      <c r="C38" s="64"/>
       <c r="D38" s="50"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="50"/>
-      <c r="B39" s="67" t="s">
+      <c r="B39" s="64" t="s">
         <v>262</v>
       </c>
-      <c r="C39" s="67"/>
+      <c r="C39" s="64"/>
       <c r="D39" s="50"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="50"/>
-      <c r="B40" s="68" t="s">
+      <c r="B40" s="77" t="s">
         <v>235</v>
       </c>
-      <c r="C40" s="68"/>
+      <c r="C40" s="77"/>
       <c r="D40" s="50"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="50"/>
-      <c r="B41" s="67" t="s">
+      <c r="B41" s="64" t="s">
         <v>236</v>
       </c>
-      <c r="C41" s="67"/>
+      <c r="C41" s="64"/>
       <c r="D41" s="50"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="50"/>
-      <c r="B42" s="67" t="s">
+      <c r="B42" s="64" t="s">
         <v>237</v>
       </c>
-      <c r="C42" s="67"/>
+      <c r="C42" s="64"/>
       <c r="D42" s="50"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="50"/>
-      <c r="B43" s="67" t="s">
+      <c r="B43" s="64" t="s">
         <v>238</v>
       </c>
-      <c r="C43" s="67"/>
+      <c r="C43" s="64"/>
       <c r="D43" s="50"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="50"/>
-      <c r="B44" s="67"/>
-      <c r="C44" s="67"/>
+      <c r="B44" s="64"/>
+      <c r="C44" s="64"/>
       <c r="D44" s="50"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="50"/>
-      <c r="B45" s="70" t="s">
+      <c r="B45" s="69" t="s">
         <v>239</v>
       </c>
-      <c r="C45" s="70"/>
+      <c r="C45" s="69"/>
       <c r="D45" s="50"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="50"/>
-      <c r="B46" s="67" t="s">
+      <c r="B46" s="64" t="s">
         <v>240</v>
       </c>
-      <c r="C46" s="67"/>
+      <c r="C46" s="64"/>
       <c r="D46" s="50"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="50"/>
-      <c r="B47" s="69" t="s">
+      <c r="B47" s="67" t="s">
         <v>263</v>
       </c>
-      <c r="C47" s="67"/>
+      <c r="C47" s="64"/>
       <c r="D47" s="50"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="50"/>
-      <c r="B48" s="67" t="s">
+      <c r="B48" s="64" t="s">
         <v>244</v>
       </c>
-      <c r="C48" s="67"/>
+      <c r="C48" s="64"/>
       <c r="D48" s="50"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="50"/>
-      <c r="B49" s="69" t="s">
+      <c r="B49" s="67" t="s">
         <v>264</v>
       </c>
-      <c r="C49" s="67"/>
+      <c r="C49" s="64"/>
       <c r="D49" s="50"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="50"/>
-      <c r="B50" s="67" t="s">
+      <c r="B50" s="64" t="s">
         <v>243</v>
       </c>
-      <c r="C50" s="67"/>
+      <c r="C50" s="64"/>
       <c r="D50" s="50"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="50"/>
-      <c r="B51" s="69" t="s">
+      <c r="B51" s="67" t="s">
         <v>265</v>
       </c>
-      <c r="C51" s="67"/>
+      <c r="C51" s="64"/>
       <c r="D51" s="50"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="50"/>
-      <c r="B52" s="67" t="s">
+      <c r="B52" s="64" t="s">
         <v>242</v>
       </c>
-      <c r="C52" s="67"/>
+      <c r="C52" s="64"/>
       <c r="D52" s="50"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="50"/>
-      <c r="B53" s="69" t="s">
+      <c r="B53" s="67" t="s">
         <v>266</v>
       </c>
-      <c r="C53" s="67"/>
+      <c r="C53" s="64"/>
       <c r="D53" s="50"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="50"/>
-      <c r="B54" s="67" t="s">
+      <c r="B54" s="64" t="s">
         <v>241</v>
       </c>
-      <c r="C54" s="67"/>
+      <c r="C54" s="64"/>
       <c r="D54" s="50"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="50"/>
-      <c r="B55" s="67"/>
-      <c r="C55" s="67"/>
+      <c r="B55" s="64"/>
+      <c r="C55" s="64"/>
       <c r="D55" s="50"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="50"/>
-      <c r="B56" s="70" t="s">
+      <c r="B56" s="69" t="s">
         <v>250</v>
       </c>
-      <c r="C56" s="70"/>
+      <c r="C56" s="69"/>
       <c r="D56" s="50"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="50"/>
-      <c r="B57" s="67" t="s">
+      <c r="B57" s="64" t="s">
         <v>251</v>
       </c>
-      <c r="C57" s="67"/>
+      <c r="C57" s="64"/>
       <c r="D57" s="50"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="50"/>
-      <c r="B58" s="67" t="s">
+      <c r="B58" s="64" t="s">
         <v>252</v>
       </c>
-      <c r="C58" s="67"/>
+      <c r="C58" s="64"/>
       <c r="D58" s="50"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -46045,69 +46045,109 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="50"/>
-      <c r="B60" s="67"/>
-      <c r="C60" s="67"/>
+      <c r="B60" s="64"/>
+      <c r="C60" s="64"/>
       <c r="D60" s="50"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="50"/>
-      <c r="B61" s="70" t="s">
+      <c r="B61" s="69" t="s">
         <v>249</v>
       </c>
-      <c r="C61" s="70"/>
+      <c r="C61" s="69"/>
       <c r="D61" s="50"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="50"/>
-      <c r="B62" s="67" t="s">
+      <c r="B62" s="64" t="s">
         <v>245</v>
       </c>
-      <c r="C62" s="67"/>
+      <c r="C62" s="64"/>
       <c r="D62" s="50"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="50"/>
-      <c r="B63" s="67" t="s">
+      <c r="B63" s="64" t="s">
         <v>246</v>
       </c>
-      <c r="C63" s="67"/>
+      <c r="C63" s="64"/>
       <c r="D63" s="50"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="50"/>
-      <c r="B64" s="67" t="s">
+      <c r="B64" s="64" t="s">
         <v>247</v>
       </c>
-      <c r="C64" s="67"/>
+      <c r="C64" s="64"/>
       <c r="D64" s="50"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="50"/>
-      <c r="B65" s="67" t="s">
+      <c r="B65" s="64" t="s">
         <v>248</v>
       </c>
-      <c r="C65" s="67"/>
+      <c r="C65" s="64"/>
       <c r="D65" s="50"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="50"/>
-      <c r="B66" s="64"/>
-      <c r="C66" s="64"/>
+      <c r="B66" s="74"/>
+      <c r="C66" s="74"/>
       <c r="D66" s="50"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B67" s="54"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="67"/>
-      <c r="C70" s="67"/>
+      <c r="B70" s="64"/>
+      <c r="C70" s="64"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="67"/>
-      <c r="C71" s="67"/>
+      <c r="B71" s="64"/>
+      <c r="C71" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B70:C70"/>
     <mergeCell ref="B71:C71"/>
     <mergeCell ref="B29:C29"/>
@@ -46124,46 +46164,6 @@
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -46321,7 +46321,7 @@
       <c r="E7" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G7" s="67"/>
+      <c r="G7" s="64"/>
       <c r="I7" s="59"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -46329,7 +46329,7 @@
       <c r="E8" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="G8" s="67"/>
+      <c r="G8" s="64"/>
       <c r="I8" s="59"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -46409,7 +46409,7 @@
       <c r="E13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="67"/>
+      <c r="G13" s="64"/>
       <c r="I13" s="59"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -46905,7 +46905,7 @@
       <c r="E37" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G37" s="67"/>
+      <c r="G37" s="64"/>
       <c r="I37" s="59"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -46913,7 +46913,7 @@
       <c r="E38" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G38" s="67"/>
+      <c r="G38" s="64"/>
       <c r="I38" s="59"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -46921,7 +46921,7 @@
       <c r="E39" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G39" s="67"/>
+      <c r="G39" s="64"/>
       <c r="I39" s="59"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -46929,7 +46929,7 @@
       <c r="E40" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G40" s="67"/>
+      <c r="G40" s="64"/>
       <c r="I40" s="59"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -46997,7 +46997,7 @@
       <c r="F44" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="G44" s="67"/>
+      <c r="G44" s="64"/>
       <c r="I44" s="59"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -47008,7 +47008,7 @@
       <c r="F45" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="G45" s="67"/>
+      <c r="G45" s="64"/>
       <c r="I45" s="59"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -47243,7 +47243,7 @@
       <c r="E57" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="G57" s="67"/>
+      <c r="G57" s="64"/>
       <c r="I57" s="59"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -47251,7 +47251,7 @@
       <c r="E58" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G58" s="67"/>
+      <c r="G58" s="64"/>
       <c r="I58" s="59"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -47259,7 +47259,7 @@
       <c r="E59" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="G59" s="67"/>
+      <c r="G59" s="64"/>
       <c r="I59" s="59"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -47267,7 +47267,7 @@
       <c r="E60" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="G60" s="67"/>
+      <c r="G60" s="64"/>
       <c r="I60" s="59"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -47275,7 +47275,7 @@
       <c r="E61" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="G61" s="67"/>
+      <c r="G61" s="64"/>
       <c r="I61" s="59"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -47283,7 +47283,7 @@
       <c r="E62" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="G62" s="67"/>
+      <c r="G62" s="64"/>
       <c r="I62" s="59"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -47493,7 +47493,7 @@
       <c r="F73" s="39" t="s">
         <v>218</v>
       </c>
-      <c r="G73" s="67"/>
+      <c r="G73" s="64"/>
       <c r="I73" s="59"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -47504,7 +47504,7 @@
       <c r="F74" s="39" t="s">
         <v>216</v>
       </c>
-      <c r="G74" s="67"/>
+      <c r="G74" s="64"/>
       <c r="I74" s="59"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -47686,7 +47686,7 @@
   <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" zoomScalePageLayoutView="88" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.19921875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -48036,7 +48036,7 @@
         <v>75</v>
       </c>
       <c r="B48">
-        <v>100</v>
+        <v>-100</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -48211,7 +48211,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -48438,7 +48438,7 @@
         <v>48</v>
       </c>
       <c r="E9" s="2">
-        <v>0.2</v>
+        <v>5</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="1"/>
@@ -48459,7 +48459,7 @@
         <v>48</v>
       </c>
       <c r="E10" s="2">
-        <v>0.1</v>
+        <v>7</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="1"/>
@@ -49011,7 +49011,7 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -49740,15 +49740,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="a656bf76-cca4-4796-b3e3-9ff4debad9ca">
@@ -49757,6 +49748,15 @@
     <TaxCatchAll xmlns="3f4d043c-ef99-408b-9086-307465b47223" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -49779,14 +49779,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80A89352-0353-48F1-9429-0E3BD72B2E30}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D351F7AA-766C-4547-802C-9F4B7AB5F83E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -49801,4 +49793,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80A89352-0353-48F1-9429-0E3BD72B2E30}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>